<commit_message>
Add to code on triple interactions and minor formatting
</commit_message>
<xml_diff>
--- a/output/lnUSDummyModelTripleInteraction.xlsx
+++ b/output/lnUSDummyModelTripleInteraction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bz22\Desktop\ComparativeMortality\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047E6191-1E40-428F-B7AC-B4798F7C63F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514C60BB-214F-44A7-B0E0-4FBEDA8A1E6D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="277">
   <si>
     <t>est1</t>
   </si>
@@ -4371,16 +4371,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>14286</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>138111</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>247651</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>1638301</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4408,15 +4408,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2343150</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>157161</xdr:rowOff>
+      <xdr:colOff>1838325</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>109536</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4743,7 +4743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
@@ -5903,7 +5903,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F261"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Redo Triple Interaction Models with proper lag variable/cohort control
</commit_message>
<xml_diff>
--- a/output/lnUSDummyModelTripleInteraction.xlsx
+++ b/output/lnUSDummyModelTripleInteraction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bz22\Desktop\ComparativeMortality\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514C60BB-214F-44A7-B0E0-4FBEDA8A1E6D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E0E31AE-757B-4876-8AE1-27D67C346CC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4371,16 +4371,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>138111</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1143000</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>14286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>1638301</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>390526</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4407,16 +4407,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1838325</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>109536</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>176211</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1247775</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4743,8 +4743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4:Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>